<commit_message>
ajout fichier + ARAVO_cluster
</commit_message>
<xml_diff>
--- a/Rstudio/final_salix_herb.xlsx
+++ b/Rstudio/final_salix_herb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apollinesaint-pierre/Desktop/SEAM_Aravo/Rstudio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68403812-0FFD-774C-91A1-80FE7D66A665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FF6E05-B936-114B-8EC7-5B02677E40AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="1160" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1859,7 +1859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F778"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A737" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A748" workbookViewId="0">
       <selection activeCell="H753" sqref="H753"/>
     </sheetView>
   </sheetViews>

</xml_diff>